<commit_message>
Creating analysis with diagramas
</commit_message>
<xml_diff>
--- a/administration.xlsx
+++ b/administration.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Niuta\Documents\Develop\python\Lab7\miniptoject2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0DB8DE0-F842-4A93-999D-3C3710BDAC8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E32217E-9BE6-430D-9631-44B4652137EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{CAD8A04A-432B-44E5-B2C8-7A217A2393A8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{CAD8A04A-432B-44E5-B2C8-7A217A2393A8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,50 +36,34 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
   <si>
-    <t>райони/districts</t>
+    <t>-</t>
   </si>
   <si>
-    <t>об'єднані територіальні громади/      united territorial community</t>
+    <t>райони</t>
   </si>
   <si>
-    <t>міста/cities</t>
+    <t>міста</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">з них міста спеціального статусу,  республі-канського, обласного значення/of which cities  with special status,   republican and regional importance   </t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-        <charset val="204"/>
-      </rPr>
-      <t xml:space="preserve">  </t>
-    </r>
+    <t>селища міського типу</t>
   </si>
   <si>
-    <t>райони в містах/city districts</t>
+    <t>сільські населені пункти</t>
   </si>
   <si>
-    <t>селища міського типу/settlements</t>
+    <t>Рік</t>
   </si>
   <si>
-    <t>сільські населені пункти/rural settle ments</t>
-  </si>
-  <si>
-    <t>-</t>
+    <t>з них міста спеціального статусу</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -96,14 +80,6 @@
       <charset val="204"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Verdana"/>
-      <family val="2"/>
-      <charset val="204"/>
-    </font>
-    <font>
-      <vertAlign val="superscript"/>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Verdana"/>
@@ -334,7 +310,7 @@
   </cellStyleXfs>
   <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -343,59 +319,59 @@
     <xf numFmtId="3" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -711,963 +687,767 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A21A7D44-5D97-4CCC-B5F3-01D2D47C84DA}">
-  <dimension ref="A1:I35"/>
+  <dimension ref="A1:G35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="13"/>
-      <c r="B1" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="16"/>
-      <c r="D1" s="19" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="C1" s="12"/>
+      <c r="D1" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="E1" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" s="11" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="14"/>
-      <c r="B2" s="17"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="10"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="13"/>
       <c r="F2" s="17"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="12"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G2" s="19"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>1990</v>
       </c>
-      <c r="B3" s="6">
+      <c r="B3" s="7">
         <v>479</v>
       </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="2" t="s">
-        <v>7</v>
+      <c r="C3" s="8"/>
+      <c r="D3" s="2">
+        <v>436</v>
       </c>
       <c r="E3" s="2">
-        <v>436</v>
-      </c>
-      <c r="F3" s="2">
         <v>145</v>
       </c>
+      <c r="F3" s="3">
+        <v>927</v>
+      </c>
       <c r="G3" s="3">
-        <v>120</v>
-      </c>
-      <c r="H3" s="3">
-        <v>927</v>
-      </c>
-      <c r="I3" s="3">
         <v>28804</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>1991</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="7">
         <v>481</v>
       </c>
-      <c r="C4" s="7"/>
-      <c r="D4" s="2" t="s">
-        <v>7</v>
+      <c r="C4" s="8"/>
+      <c r="D4" s="2">
+        <v>436</v>
       </c>
       <c r="E4" s="2">
-        <v>436</v>
+        <v>149</v>
       </c>
       <c r="F4" s="2">
-        <v>149</v>
+        <v>925</v>
       </c>
       <c r="G4" s="2">
-        <v>120</v>
-      </c>
-      <c r="H4" s="2">
-        <v>925</v>
-      </c>
-      <c r="I4" s="2">
         <v>28845</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>1992</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="7">
         <v>485</v>
       </c>
-      <c r="C5" s="7"/>
-      <c r="D5" s="2" t="s">
-        <v>7</v>
+      <c r="C5" s="8"/>
+      <c r="D5" s="2">
+        <v>437</v>
       </c>
       <c r="E5" s="2">
-        <v>437</v>
+        <v>153</v>
       </c>
       <c r="F5" s="2">
-        <v>153</v>
+        <v>923</v>
       </c>
       <c r="G5" s="2">
-        <v>120</v>
-      </c>
-      <c r="H5" s="2">
-        <v>923</v>
-      </c>
-      <c r="I5" s="2">
         <v>28828</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>1993</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="7">
         <v>486</v>
       </c>
-      <c r="C6" s="7"/>
-      <c r="D6" s="2" t="s">
-        <v>7</v>
+      <c r="C6" s="8"/>
+      <c r="D6" s="2">
+        <v>441</v>
       </c>
       <c r="E6" s="2">
-        <v>441</v>
+        <v>158</v>
       </c>
       <c r="F6" s="2">
-        <v>158</v>
+        <v>915</v>
       </c>
       <c r="G6" s="2">
-        <v>120</v>
-      </c>
-      <c r="H6" s="2">
-        <v>915</v>
-      </c>
-      <c r="I6" s="2">
         <v>28858</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>1994</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7" s="7">
         <v>489</v>
       </c>
-      <c r="C7" s="7"/>
-      <c r="D7" s="2" t="s">
-        <v>7</v>
+      <c r="C7" s="8"/>
+      <c r="D7" s="2">
+        <v>445</v>
       </c>
       <c r="E7" s="2">
-        <v>445</v>
+        <v>164</v>
       </c>
       <c r="F7" s="2">
-        <v>164</v>
+        <v>911</v>
       </c>
       <c r="G7" s="2">
-        <v>120</v>
-      </c>
-      <c r="H7" s="2">
-        <v>911</v>
-      </c>
-      <c r="I7" s="2">
         <v>28863</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>1995</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B8" s="7">
         <v>489</v>
       </c>
-      <c r="C8" s="7"/>
-      <c r="D8" s="2" t="s">
-        <v>7</v>
+      <c r="C8" s="8"/>
+      <c r="D8" s="2">
+        <v>445</v>
       </c>
       <c r="E8" s="2">
-        <v>445</v>
+        <v>165</v>
       </c>
       <c r="F8" s="2">
-        <v>165</v>
+        <v>909</v>
       </c>
       <c r="G8" s="2">
-        <v>120</v>
-      </c>
-      <c r="H8" s="2">
-        <v>909</v>
-      </c>
-      <c r="I8" s="2">
         <v>28864</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>1996</v>
       </c>
-      <c r="B9" s="6">
-        <v>490</v>
-      </c>
-      <c r="C9" s="7"/>
-      <c r="D9" s="2" t="s">
-        <v>7</v>
+      <c r="B9" s="7">
+        <v>490</v>
+      </c>
+      <c r="C9" s="8"/>
+      <c r="D9" s="2">
+        <v>446</v>
       </c>
       <c r="E9" s="2">
-        <v>446</v>
+        <v>167</v>
       </c>
       <c r="F9" s="2">
-        <v>167</v>
+        <v>907</v>
       </c>
       <c r="G9" s="2">
-        <v>121</v>
-      </c>
-      <c r="H9" s="2">
-        <v>907</v>
-      </c>
-      <c r="I9" s="2">
         <v>28838</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>1997</v>
       </c>
-      <c r="B10" s="6">
-        <v>490</v>
-      </c>
-      <c r="C10" s="7"/>
-      <c r="D10" s="2" t="s">
-        <v>7</v>
+      <c r="B10" s="7">
+        <v>490</v>
+      </c>
+      <c r="C10" s="8"/>
+      <c r="D10" s="2">
+        <v>447</v>
       </c>
       <c r="E10" s="2">
-        <v>447</v>
+        <v>167</v>
       </c>
       <c r="F10" s="2">
-        <v>167</v>
+        <v>904</v>
       </c>
       <c r="G10" s="2">
-        <v>121</v>
-      </c>
-      <c r="H10" s="2">
-        <v>904</v>
-      </c>
-      <c r="I10" s="2">
         <v>28834</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>1998</v>
       </c>
-      <c r="B11" s="6">
-        <v>490</v>
-      </c>
-      <c r="C11" s="7"/>
-      <c r="D11" s="2" t="s">
-        <v>7</v>
+      <c r="B11" s="7">
+        <v>490</v>
+      </c>
+      <c r="C11" s="8"/>
+      <c r="D11" s="2">
+        <v>448</v>
       </c>
       <c r="E11" s="2">
-        <v>448</v>
+        <v>168</v>
       </c>
       <c r="F11" s="2">
-        <v>168</v>
+        <v>896</v>
       </c>
       <c r="G11" s="2">
-        <v>121</v>
-      </c>
-      <c r="H11" s="2">
-        <v>896</v>
-      </c>
-      <c r="I11" s="2">
         <v>28794</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>1999</v>
       </c>
-      <c r="B12" s="6">
-        <v>490</v>
-      </c>
-      <c r="C12" s="7"/>
-      <c r="D12" s="2" t="s">
-        <v>7</v>
+      <c r="B12" s="7">
+        <v>490</v>
+      </c>
+      <c r="C12" s="8"/>
+      <c r="D12" s="2">
+        <v>448</v>
       </c>
       <c r="E12" s="2">
-        <v>448</v>
+        <v>169</v>
       </c>
       <c r="F12" s="2">
-        <v>169</v>
+        <v>897</v>
       </c>
       <c r="G12" s="2">
-        <v>121</v>
-      </c>
-      <c r="H12" s="2">
-        <v>897</v>
-      </c>
-      <c r="I12" s="2">
         <v>28775</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>2000</v>
       </c>
-      <c r="B13" s="6">
-        <v>490</v>
-      </c>
-      <c r="C13" s="7"/>
-      <c r="D13" s="2" t="s">
-        <v>7</v>
+      <c r="B13" s="7">
+        <v>490</v>
+      </c>
+      <c r="C13" s="8"/>
+      <c r="D13" s="2">
+        <v>448</v>
       </c>
       <c r="E13" s="2">
-        <v>448</v>
+        <v>170</v>
       </c>
       <c r="F13" s="2">
-        <v>170</v>
+        <v>894</v>
       </c>
       <c r="G13" s="2">
-        <v>121</v>
-      </c>
-      <c r="H13" s="2">
-        <v>894</v>
-      </c>
-      <c r="I13" s="2">
         <v>28739</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>2001</v>
       </c>
-      <c r="B14" s="6">
-        <v>490</v>
-      </c>
-      <c r="C14" s="7"/>
-      <c r="D14" s="2" t="s">
-        <v>7</v>
+      <c r="B14" s="7">
+        <v>490</v>
+      </c>
+      <c r="C14" s="8"/>
+      <c r="D14" s="2">
+        <v>451</v>
       </c>
       <c r="E14" s="2">
-        <v>451</v>
+        <v>173</v>
       </c>
       <c r="F14" s="2">
-        <v>173</v>
+        <v>893</v>
       </c>
       <c r="G14" s="2">
-        <v>122</v>
-      </c>
-      <c r="H14" s="2">
-        <v>893</v>
-      </c>
-      <c r="I14" s="2">
         <v>28651</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>2002</v>
       </c>
-      <c r="B15" s="6">
-        <v>490</v>
-      </c>
-      <c r="C15" s="7"/>
-      <c r="D15" s="2" t="s">
-        <v>7</v>
+      <c r="B15" s="7">
+        <v>490</v>
+      </c>
+      <c r="C15" s="8"/>
+      <c r="D15" s="2">
+        <v>454</v>
       </c>
       <c r="E15" s="2">
-        <v>454</v>
+        <v>174</v>
       </c>
       <c r="F15" s="2">
-        <v>174</v>
+        <v>889</v>
       </c>
       <c r="G15" s="2">
-        <v>118</v>
-      </c>
-      <c r="H15" s="2">
-        <v>889</v>
-      </c>
-      <c r="I15" s="2">
         <v>28619</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>2003</v>
       </c>
-      <c r="B16" s="6">
-        <v>490</v>
-      </c>
-      <c r="C16" s="7"/>
-      <c r="D16" s="2" t="s">
-        <v>7</v>
+      <c r="B16" s="7">
+        <v>490</v>
+      </c>
+      <c r="C16" s="8"/>
+      <c r="D16" s="2">
+        <v>453</v>
       </c>
       <c r="E16" s="2">
-        <v>453</v>
+        <v>176</v>
       </c>
       <c r="F16" s="2">
-        <v>176</v>
+        <v>887</v>
       </c>
       <c r="G16" s="2">
-        <v>118</v>
-      </c>
-      <c r="H16" s="2">
-        <v>887</v>
-      </c>
-      <c r="I16" s="2">
         <v>28612</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>2004</v>
       </c>
-      <c r="B17" s="6">
-        <v>490</v>
-      </c>
-      <c r="C17" s="7"/>
-      <c r="D17" s="2" t="s">
-        <v>7</v>
+      <c r="B17" s="7">
+        <v>490</v>
+      </c>
+      <c r="C17" s="8"/>
+      <c r="D17" s="2">
+        <v>455</v>
       </c>
       <c r="E17" s="2">
-        <v>455</v>
+        <v>178</v>
       </c>
       <c r="F17" s="2">
-        <v>178</v>
+        <v>886</v>
       </c>
       <c r="G17" s="2">
-        <v>118</v>
-      </c>
-      <c r="H17" s="2">
-        <v>886</v>
-      </c>
-      <c r="I17" s="2">
         <v>28597</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>2005</v>
       </c>
-      <c r="B18" s="6">
-        <v>490</v>
-      </c>
-      <c r="C18" s="7"/>
-      <c r="D18" s="2" t="s">
-        <v>7</v>
+      <c r="B18" s="7">
+        <v>490</v>
+      </c>
+      <c r="C18" s="8"/>
+      <c r="D18" s="2">
+        <v>456</v>
       </c>
       <c r="E18" s="2">
-        <v>456</v>
+        <v>178</v>
       </c>
       <c r="F18" s="2">
-        <v>178</v>
+        <v>886</v>
       </c>
       <c r="G18" s="2">
-        <v>118</v>
-      </c>
-      <c r="H18" s="2">
-        <v>886</v>
-      </c>
-      <c r="I18" s="2">
         <v>28585</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>2006</v>
       </c>
-      <c r="B19" s="6">
-        <v>490</v>
-      </c>
-      <c r="C19" s="7"/>
-      <c r="D19" s="2" t="s">
-        <v>7</v>
+      <c r="B19" s="7">
+        <v>490</v>
+      </c>
+      <c r="C19" s="8"/>
+      <c r="D19" s="2">
+        <v>457</v>
       </c>
       <c r="E19" s="2">
-        <v>457</v>
+        <v>178</v>
       </c>
       <c r="F19" s="2">
-        <v>178</v>
+        <v>885</v>
       </c>
       <c r="G19" s="2">
-        <v>118</v>
-      </c>
-      <c r="H19" s="2">
-        <v>885</v>
-      </c>
-      <c r="I19" s="2">
         <v>28562</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>2007</v>
       </c>
-      <c r="B20" s="6">
-        <v>490</v>
-      </c>
-      <c r="C20" s="7"/>
-      <c r="D20" s="2" t="s">
-        <v>7</v>
+      <c r="B20" s="7">
+        <v>490</v>
+      </c>
+      <c r="C20" s="8"/>
+      <c r="D20" s="2">
+        <v>458</v>
       </c>
       <c r="E20" s="2">
-        <v>458</v>
+        <v>179</v>
       </c>
       <c r="F20" s="2">
-        <v>179</v>
+        <v>886</v>
       </c>
       <c r="G20" s="2">
-        <v>118</v>
-      </c>
-      <c r="H20" s="2">
-        <v>886</v>
-      </c>
-      <c r="I20" s="2">
         <v>28540</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>2008</v>
       </c>
-      <c r="B21" s="6">
-        <v>490</v>
-      </c>
-      <c r="C21" s="7"/>
-      <c r="D21" s="2" t="s">
-        <v>7</v>
+      <c r="B21" s="7">
+        <v>490</v>
+      </c>
+      <c r="C21" s="8"/>
+      <c r="D21" s="2">
+        <v>458</v>
       </c>
       <c r="E21" s="2">
-        <v>458</v>
+        <v>179</v>
       </c>
       <c r="F21" s="2">
-        <v>179</v>
+        <v>886</v>
       </c>
       <c r="G21" s="2">
-        <v>118</v>
-      </c>
-      <c r="H21" s="2">
-        <v>886</v>
-      </c>
-      <c r="I21" s="2">
         <v>28504</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>2009</v>
       </c>
-      <c r="B22" s="6">
-        <v>490</v>
-      </c>
-      <c r="C22" s="7"/>
-      <c r="D22" s="2" t="s">
-        <v>7</v>
+      <c r="B22" s="7">
+        <v>490</v>
+      </c>
+      <c r="C22" s="8"/>
+      <c r="D22" s="2">
+        <v>459</v>
       </c>
       <c r="E22" s="2">
-        <v>459</v>
+        <v>179</v>
       </c>
       <c r="F22" s="2">
-        <v>179</v>
+        <v>886</v>
       </c>
       <c r="G22" s="2">
-        <v>118</v>
-      </c>
-      <c r="H22" s="2">
-        <v>886</v>
-      </c>
-      <c r="I22" s="2">
         <v>28490</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>2010</v>
       </c>
-      <c r="B23" s="6">
-        <v>490</v>
-      </c>
-      <c r="C23" s="7"/>
-      <c r="D23" s="2" t="s">
-        <v>7</v>
+      <c r="B23" s="7">
+        <v>490</v>
+      </c>
+      <c r="C23" s="8"/>
+      <c r="D23" s="2">
+        <v>459</v>
       </c>
       <c r="E23" s="2">
-        <v>459</v>
+        <v>179</v>
       </c>
       <c r="F23" s="2">
-        <v>179</v>
+        <v>885</v>
       </c>
       <c r="G23" s="2">
-        <v>118</v>
-      </c>
-      <c r="H23" s="2">
-        <v>885</v>
-      </c>
-      <c r="I23" s="2">
         <v>28471</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>2011</v>
       </c>
-      <c r="B24" s="6">
-        <v>490</v>
-      </c>
-      <c r="C24" s="7"/>
-      <c r="D24" s="2" t="s">
-        <v>7</v>
+      <c r="B24" s="7">
+        <v>490</v>
+      </c>
+      <c r="C24" s="8"/>
+      <c r="D24" s="2">
+        <v>459</v>
       </c>
       <c r="E24" s="2">
-        <v>459</v>
+        <v>180</v>
       </c>
       <c r="F24" s="2">
-        <v>180</v>
+        <v>885</v>
       </c>
       <c r="G24" s="2">
-        <v>118</v>
-      </c>
-      <c r="H24" s="2">
-        <v>885</v>
-      </c>
-      <c r="I24" s="2">
         <v>28457</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>2012</v>
       </c>
-      <c r="B25" s="6">
-        <v>490</v>
-      </c>
-      <c r="C25" s="7"/>
-      <c r="D25" s="2" t="s">
-        <v>7</v>
+      <c r="B25" s="7">
+        <v>490</v>
+      </c>
+      <c r="C25" s="8"/>
+      <c r="D25" s="2">
+        <v>459</v>
       </c>
       <c r="E25" s="2">
-        <v>459</v>
+        <v>180</v>
       </c>
       <c r="F25" s="2">
-        <v>180</v>
+        <v>885</v>
       </c>
       <c r="G25" s="2">
-        <v>114</v>
-      </c>
-      <c r="H25" s="2">
-        <v>885</v>
-      </c>
-      <c r="I25" s="2">
         <v>28450</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>2013</v>
       </c>
-      <c r="B26" s="6">
-        <v>490</v>
-      </c>
-      <c r="C26" s="7"/>
-      <c r="D26" s="2" t="s">
-        <v>7</v>
+      <c r="B26" s="7">
+        <v>490</v>
+      </c>
+      <c r="C26" s="8"/>
+      <c r="D26" s="2">
+        <v>460</v>
       </c>
       <c r="E26" s="2">
-        <v>460</v>
+        <v>180</v>
       </c>
       <c r="F26" s="2">
-        <v>180</v>
+        <v>885</v>
       </c>
       <c r="G26" s="2">
-        <v>111</v>
-      </c>
-      <c r="H26" s="2">
-        <v>885</v>
-      </c>
-      <c r="I26" s="2">
         <v>28441</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>2014</v>
       </c>
-      <c r="B27" s="6">
-        <v>490</v>
-      </c>
-      <c r="C27" s="7"/>
-      <c r="D27" s="2" t="s">
-        <v>7</v>
+      <c r="B27" s="7">
+        <v>490</v>
+      </c>
+      <c r="C27" s="8"/>
+      <c r="D27" s="2">
+        <v>460</v>
       </c>
       <c r="E27" s="2">
-        <v>460</v>
+        <v>182</v>
       </c>
       <c r="F27" s="2">
-        <v>182</v>
+        <v>885</v>
       </c>
       <c r="G27" s="2">
-        <v>111</v>
-      </c>
-      <c r="H27" s="2">
-        <v>885</v>
-      </c>
-      <c r="I27" s="2">
         <v>28397</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>2015</v>
       </c>
-      <c r="B28" s="6">
-        <v>490</v>
-      </c>
-      <c r="C28" s="7"/>
-      <c r="D28" s="2" t="s">
-        <v>7</v>
+      <c r="B28" s="7">
+        <v>490</v>
+      </c>
+      <c r="C28" s="8"/>
+      <c r="D28" s="2">
+        <v>460</v>
       </c>
       <c r="E28" s="2">
-        <v>460</v>
+        <v>184</v>
       </c>
       <c r="F28" s="2">
-        <v>184</v>
+        <v>885</v>
       </c>
       <c r="G28" s="2">
-        <v>111</v>
-      </c>
-      <c r="H28" s="2">
-        <v>885</v>
-      </c>
-      <c r="I28" s="2">
         <v>28388</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>2016</v>
       </c>
-      <c r="B29" s="6">
-        <v>490</v>
-      </c>
-      <c r="C29" s="7"/>
+      <c r="B29" s="7">
+        <v>490</v>
+      </c>
+      <c r="C29" s="8"/>
       <c r="D29" s="2">
-        <v>93</v>
+        <v>460</v>
       </c>
       <c r="E29" s="2">
-        <v>460</v>
+        <v>187</v>
       </c>
       <c r="F29" s="2">
-        <v>187</v>
+        <v>885</v>
       </c>
       <c r="G29" s="2">
-        <v>111</v>
-      </c>
-      <c r="H29" s="2">
-        <v>885</v>
-      </c>
-      <c r="I29" s="2">
         <v>28385</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="4">
         <v>2017</v>
       </c>
-      <c r="B30" s="8">
-        <v>490</v>
-      </c>
-      <c r="C30" s="9"/>
+      <c r="B30" s="20">
+        <v>490</v>
+      </c>
+      <c r="C30" s="21"/>
       <c r="D30" s="5">
-        <v>216</v>
+        <v>460</v>
       </c>
       <c r="E30" s="5">
-        <v>460</v>
+        <v>189</v>
       </c>
       <c r="F30" s="5">
-        <v>189</v>
+        <v>885</v>
       </c>
       <c r="G30" s="5">
-        <v>111</v>
-      </c>
-      <c r="H30" s="5">
-        <v>885</v>
-      </c>
-      <c r="I30" s="5">
         <v>28377</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>2018</v>
       </c>
-      <c r="B31" s="6">
-        <v>490</v>
-      </c>
-      <c r="C31" s="7"/>
+      <c r="B31" s="7">
+        <v>490</v>
+      </c>
+      <c r="C31" s="8"/>
       <c r="D31" s="2">
-        <v>458</v>
+        <v>461</v>
       </c>
       <c r="E31" s="2">
-        <v>461</v>
+        <v>189</v>
       </c>
       <c r="F31" s="2">
-        <v>189</v>
+        <v>883</v>
       </c>
       <c r="G31" s="2">
-        <v>108</v>
-      </c>
-      <c r="H31" s="2">
-        <v>883</v>
-      </c>
-      <c r="I31" s="2">
         <v>28378</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>2019</v>
       </c>
-      <c r="B32" s="6">
-        <v>490</v>
-      </c>
-      <c r="C32" s="7"/>
+      <c r="B32" s="7">
+        <v>490</v>
+      </c>
+      <c r="C32" s="8"/>
       <c r="D32" s="2">
-        <v>686</v>
+        <v>461</v>
       </c>
       <c r="E32" s="2">
-        <v>461</v>
+        <v>189</v>
       </c>
       <c r="F32" s="2">
-        <v>189</v>
+        <v>883</v>
       </c>
       <c r="G32" s="2">
-        <v>108</v>
-      </c>
-      <c r="H32" s="2">
-        <v>883</v>
-      </c>
-      <c r="I32" s="2">
         <v>28376</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>2020</v>
       </c>
-      <c r="B33" s="6">
-        <v>490</v>
-      </c>
-      <c r="C33" s="7"/>
+      <c r="B33" s="7">
+        <v>490</v>
+      </c>
+      <c r="C33" s="8"/>
       <c r="D33" s="2">
-        <v>841</v>
+        <v>461</v>
       </c>
       <c r="E33" s="2">
+        <v>189</v>
+      </c>
+      <c r="F33" s="2">
+        <v>882</v>
+      </c>
+      <c r="G33" s="2">
+        <v>28376</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A34" s="6">
+        <v>2021</v>
+      </c>
+      <c r="B34" s="7">
+        <v>140</v>
+      </c>
+      <c r="C34" s="8"/>
+      <c r="D34" s="2">
         <v>461</v>
       </c>
-      <c r="F33" s="2">
-        <v>189</v>
-      </c>
-      <c r="G33" s="2">
-        <v>108</v>
-      </c>
-      <c r="H33" s="2">
+      <c r="E34" t="s">
+        <v>0</v>
+      </c>
+      <c r="F34" s="2">
         <v>882</v>
       </c>
-      <c r="I33" s="2">
-        <v>28376</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A34" s="21">
-        <v>2021</v>
-      </c>
-      <c r="B34" s="6">
+      <c r="G34" s="2">
+        <v>28372</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A35" s="6">
+        <v>2022</v>
+      </c>
+      <c r="B35" s="7">
         <v>140</v>
       </c>
-      <c r="C34" s="7"/>
-      <c r="D34" s="2">
-        <v>1469</v>
-      </c>
-      <c r="E34" s="2">
+      <c r="C35" s="8"/>
+      <c r="D35" s="2">
         <v>461</v>
       </c>
-      <c r="F34" t="s">
-        <v>7</v>
-      </c>
-      <c r="G34" s="2">
-        <v>108</v>
-      </c>
-      <c r="H34" s="2">
-        <v>882</v>
-      </c>
-      <c r="I34" s="2">
-        <v>28372</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A35" s="21">
-        <v>2022</v>
-      </c>
-      <c r="B35" s="6">
-        <v>140</v>
-      </c>
-      <c r="C35" s="7"/>
-      <c r="D35" s="2">
-        <v>1469</v>
-      </c>
-      <c r="E35" s="2">
-        <v>461</v>
-      </c>
-      <c r="F35" t="s">
-        <v>7</v>
+      <c r="E35" t="s">
+        <v>0</v>
+      </c>
+      <c r="F35" s="2">
+        <v>881</v>
       </c>
       <c r="G35" s="2">
-        <v>108</v>
-      </c>
-      <c r="H35" s="2">
-        <v>881</v>
-      </c>
-      <c r="I35" s="2">
         <v>28369</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="41">
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:C2"/>
+  <mergeCells count="39">
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B30:C30"/>
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="E1:E2"/>
+    <mergeCell ref="B12:C12"/>
     <mergeCell ref="F1:F2"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="H1:H2"/>
-    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="G1:G2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="B6:C6"/>
-    <mergeCell ref="G1:G2"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:C2"/>
     <mergeCell ref="B24:C24"/>
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="B14:C14"/>
@@ -1679,16 +1459,6 @@
     <mergeCell ref="B20:C20"/>
     <mergeCell ref="B21:C21"/>
     <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B30:C30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>